<commit_message>
cambio unidades reducción, implementación R2, renaming módulos
</commit_message>
<xml_diff>
--- a/resultados/por_vector/U1.xlsx
+++ b/resultados/por_vector/U1.xlsx
@@ -2540,7 +2540,7 @@
         <v>-20.116107</v>
       </c>
       <c r="D7">
-        <v>-0.1630434782608696</v>
+        <v>2.820015000000001</v>
       </c>
       <c r="E7">
         <v>-0.003531000000000001</v>
@@ -2557,7 +2557,7 @@
         <v>-34.10731505385696</v>
       </c>
       <c r="D8">
-        <v>-0.04531937258489869</v>
+        <v>1.478707999999997</v>
       </c>
       <c r="E8">
         <v>-0.001776052648086699</v>
@@ -2574,7 +2574,7 @@
         <v>-12.172336</v>
       </c>
       <c r="D9">
-        <v>-0.3529411764705883</v>
+        <v>3.175392</v>
       </c>
       <c r="E9">
         <v>-0.001012</v>
@@ -2591,7 +2591,7 @@
         <v>-1608.562771378963</v>
       </c>
       <c r="D10">
-        <v>-0.01281188902398977</v>
+        <v>20.34803099999999</v>
       </c>
       <c r="E10">
         <v>-0.07217493477717785</v>
@@ -2608,7 +2608,7 @@
         <v>-57.38637873379457</v>
       </c>
       <c r="D11">
-        <v>-0.08196205340619515</v>
+        <v>4.347200000000001</v>
       </c>
       <c r="E11">
         <v>-0.01887709826769558</v>
@@ -2625,7 +2625,7 @@
         <v>-54.15982</v>
       </c>
       <c r="D12">
-        <v>-0.06699346405228757</v>
+        <v>3.400539999999999</v>
       </c>
       <c r="E12">
         <v>-0.007183</v>
@@ -2642,7 +2642,7 @@
         <v>-4924.164833998421</v>
       </c>
       <c r="D13">
-        <v>-0.002028174502138433</v>
+        <v>9.966851047481214</v>
       </c>
       <c r="E13">
         <v>-1.778318827735075</v>
@@ -2659,7 +2659,7 @@
         <v>-112.2570806532047</v>
       </c>
       <c r="D14">
-        <v>-0.05398579390682554</v>
+        <v>5.749876</v>
       </c>
       <c r="E14">
         <v>-0.01460349689777608</v>
@@ -2676,7 +2676,7 @@
         <v>-69.11241232398362</v>
       </c>
       <c r="D15">
-        <v>-0.3295084459457132</v>
+        <v>17.12898</v>
       </c>
       <c r="E15">
         <v>-0.007278821729750776</v>
@@ -2693,7 +2693,7 @@
         <v>-58.505447</v>
       </c>
       <c r="D16">
-        <v>-0.5388888888888888</v>
+        <v>20.487467</v>
       </c>
       <c r="E16">
         <v>-0.003047</v>
@@ -2710,7 +2710,7 @@
         <v>-98.46687823393545</v>
       </c>
       <c r="D17">
-        <v>-0.0402366620368898</v>
+        <v>3.808728000000002</v>
       </c>
       <c r="E17">
         <v>-0.007678327997031772</v>
@@ -2727,7 +2727,7 @@
         <v>-25.56411</v>
       </c>
       <c r="D18">
-        <v>-0.1523437499999998</v>
+        <v>3.379661999999996</v>
       </c>
       <c r="E18">
         <v>-0.003245</v>
@@ -2744,7 +2744,7 @@
         <v>-58.51437483864774</v>
       </c>
       <c r="D19">
-        <v>-0.4815467558311358</v>
+        <v>19.018912</v>
       </c>
       <c r="E19">
         <v>-0.009611428192944766</v>
@@ -2761,7 +2761,7 @@
         <v>-37.27145400000001</v>
       </c>
       <c r="D20">
-        <v>-0.2321428571428574</v>
+        <v>7.022158000000008</v>
       </c>
       <c r="E20">
         <v>-0.001518</v>
@@ -2778,7 +2778,7 @@
         <v>-5.845752</v>
       </c>
       <c r="D21">
-        <v>-0.5249999999999999</v>
+        <v>2.012472</v>
       </c>
       <c r="E21">
         <v>-0.000671</v>
@@ -2795,7 +2795,7 @@
         <v>-13.681855</v>
       </c>
       <c r="D22">
-        <v>-0.3281249999999999</v>
+        <v>3.380222999999999</v>
       </c>
       <c r="E22">
         <v>-0.0009350000000000001</v>
@@ -2812,7 +2812,7 @@
         <v>-7.127263000000001</v>
       </c>
       <c r="D23">
-        <v>-0.375</v>
+        <v>1.943799</v>
       </c>
       <c r="E23">
         <v>-0.001573</v>
@@ -2846,7 +2846,7 @@
         <v>-13.51603</v>
       </c>
       <c r="D25">
-        <v>-0.1693548387096773</v>
+        <v>1.957493999999999</v>
       </c>
       <c r="E25">
         <v>-0.001595</v>
@@ -2863,7 +2863,7 @@
         <v>-36.886388</v>
       </c>
       <c r="D26">
-        <v>-0.03985507246376813</v>
+        <v>1.413764</v>
       </c>
       <c r="E26">
         <v>-0.003157000000000001</v>
@@ -2880,7 +2880,7 @@
         <v>-15.662262</v>
       </c>
       <c r="D27">
-        <v>-0.3012820512820512</v>
+        <v>3.626237999999999</v>
       </c>
       <c r="E27">
         <v>-0.002233</v>
@@ -2897,7 +2897,7 @@
         <v>-11.27764</v>
       </c>
       <c r="D28">
-        <v>-0.1585365853658536</v>
+        <v>1.543256</v>
       </c>
       <c r="E28">
         <v>-0.00209</v>
@@ -2914,7 +2914,7 @@
         <v>-832.4596800852414</v>
       </c>
       <c r="D29">
-        <v>-0.007970003451287623</v>
+        <v>6.582245999999941</v>
       </c>
       <c r="E29">
         <v>-0.2518026860511922</v>
@@ -2931,7 +2931,7 @@
         <v>-28.71242095692438</v>
       </c>
       <c r="D30">
-        <v>-0.01776374370372243</v>
+        <v>0.5011379999999974</v>
       </c>
       <c r="E30">
         <v>-0.001260477674916562</v>
@@ -2948,7 +2948,7 @@
         <v>-1302.21413988054</v>
       </c>
       <c r="D31">
-        <v>-0.01721097675432654</v>
+        <v>22.03316500000005</v>
       </c>
       <c r="E31">
         <v>-0.2463981343198751</v>
@@ -2965,7 +2965,7 @@
         <v>-44.87191913375786</v>
       </c>
       <c r="D32">
-        <v>-0.1130281751983129</v>
+        <v>4.556750000000001</v>
       </c>
       <c r="E32">
         <v>-0.002708021673733124</v>
@@ -2982,7 +2982,7 @@
         <v>-28.063574</v>
       </c>
       <c r="D33">
-        <v>-0.53125</v>
+        <v>9.736342</v>
       </c>
       <c r="E33">
         <v>-0.001078</v>
@@ -2999,7 +2999,7 @@
         <v>-1574.722714601005</v>
       </c>
       <c r="D34">
-        <v>-0.00446148347777404</v>
+        <v>6.994393999999829</v>
       </c>
       <c r="E34">
         <v>-0.1436397623461649</v>
@@ -3016,7 +3016,7 @@
         <v>-80.135352</v>
       </c>
       <c r="D35">
-        <v>-0.08749999999999997</v>
+        <v>6.447671999999997</v>
       </c>
       <c r="E35">
         <v>-0.001914</v>
@@ -3033,7 +3033,7 @@
         <v>-350.7150493800869</v>
       </c>
       <c r="D36">
-        <v>-0.009689517202642774</v>
+        <v>3.365648000000022</v>
       </c>
       <c r="E36">
         <v>-0.05960486903128601</v>
@@ -3050,7 +3050,7 @@
         <v>-2592.414874076669</v>
       </c>
       <c r="D37">
-        <v>-0.0001846096857086565</v>
+        <v>0.4784965600301803</v>
       </c>
       <c r="E37">
         <v>-2.610689701990603</v>
@@ -3067,7 +3067,7 @@
         <v>-5112.251091638024</v>
       </c>
       <c r="D38">
-        <v>-8.559342694440841E-05</v>
+        <v>0.4375376399875677</v>
       </c>
       <c r="E38">
         <v>-5.630232479777559</v>
@@ -3084,7 +3084,7 @@
         <v>-4101.655269795333</v>
       </c>
       <c r="D39">
-        <v>-0.0001399403472995327</v>
+        <v>0.5739067502481703</v>
       </c>
       <c r="E39">
         <v>-3.443875121574587</v>
@@ -3101,7 +3101,7 @@
         <v>-2119.893996130817</v>
       </c>
       <c r="D40">
-        <v>-8.251974703942239E-05</v>
+        <v>0.1749186820657087</v>
       </c>
       <c r="E40">
         <v>-5.83992836399674</v>
@@ -3118,7 +3118,7 @@
         <v>-5844.25196652527</v>
       </c>
       <c r="D41">
-        <v>-4.699780083904553E-06</v>
+        <v>0.02746656991075724</v>
       </c>
       <c r="E41">
         <v>-102.5307362548293</v>
@@ -3135,7 +3135,7 @@
         <v>-3111.004880708113</v>
       </c>
       <c r="D42">
-        <v>-0.0003870698844344959</v>
+        <v>1.203710379613312</v>
       </c>
       <c r="E42">
         <v>-1.245398270899965</v>
@@ -3152,7 +3152,7 @@
         <v>-2587.768367111283</v>
       </c>
       <c r="D43">
-        <v>-0.0001366971922813795</v>
+        <v>0.3536923213114278</v>
       </c>
       <c r="E43">
         <v>-3.52556998244044</v>
@@ -3169,7 +3169,7 @@
         <v>-298.3828098194426</v>
       </c>
       <c r="D44">
-        <v>-0.02207664257138189</v>
+        <v>6.44500653615944</v>
       </c>
       <c r="E44">
         <v>-0.02230899512668729</v>
@@ -3186,7 +3186,7 @@
         <v>-10.60392981397204</v>
       </c>
       <c r="D45">
-        <v>-0.05620402798796533</v>
+        <v>0.5642693572966522</v>
       </c>
       <c r="E45">
         <v>-0.00905544817589414</v>
@@ -3203,7 +3203,7 @@
         <v>-1444.869774249915</v>
       </c>
       <c r="D46">
-        <v>-0.000427401038846755</v>
+        <v>0.6172750185285167</v>
       </c>
       <c r="E46">
         <v>-1.127923321038185</v>
@@ -3220,7 +3220,7 @@
         <v>-3655.776554582183</v>
       </c>
       <c r="D47">
-        <v>-0.0008968512368031367</v>
+        <v>3.275749864135832</v>
       </c>
       <c r="E47">
         <v>-0.5377723675466582</v>
@@ -3237,7 +3237,7 @@
         <v>-5013.99722629369</v>
       </c>
       <c r="D48">
-        <v>-0.0002496467050095535</v>
+        <v>1.251415474721398</v>
       </c>
       <c r="E48">
         <v>-1.930688188792334</v>
@@ -3254,7 +3254,7 @@
         <v>-3311.583833100464</v>
       </c>
       <c r="D49">
-        <v>-0.0002758181249673317</v>
+        <v>0.9131429821327401</v>
       </c>
       <c r="E49">
         <v>-1.747537642797079</v>
@@ -3271,7 +3271,7 @@
         <v>-63015.94609120856</v>
       </c>
       <c r="D50">
-        <v>-5.8345340990395E-06</v>
+        <v>0.3676665410894202</v>
       </c>
       <c r="E50">
         <v>-82.58970654155775</v>
@@ -3288,7 +3288,7 @@
         <v>-5028.86815236008</v>
       </c>
       <c r="D51">
-        <v>-0.0001426015282735596</v>
+        <v>0.7170220355747006</v>
       </c>
       <c r="E51">
         <v>-3.379615693790376</v>
@@ -3305,7 +3305,7 @@
         <v>-189.026009586411</v>
       </c>
       <c r="D52">
-        <v>-0.01259169402186927</v>
+        <v>2.350560140813883</v>
       </c>
       <c r="E52">
         <v>-0.03875071947240897</v>
@@ -3322,7 +3322,7 @@
         <v>-8350.522194616027</v>
       </c>
       <c r="D53">
-        <v>-9.170217953467421E-05</v>
+        <v>0.7656908699773339</v>
       </c>
       <c r="E53">
         <v>-5.255205912281956</v>
@@ -3339,7 +3339,7 @@
         <v>-45.42878999999999</v>
       </c>
       <c r="D54">
-        <v>-0.03571428571428557</v>
+        <v>1.566509999999994</v>
       </c>
       <c r="E54">
         <v>-0.001914</v>
@@ -3373,7 +3373,7 @@
         <v>-47.26922871060579</v>
       </c>
       <c r="D56">
-        <v>-0.002780677486551181</v>
+        <v>0.1310759999999931</v>
       </c>
       <c r="E56">
         <v>-0.003966870485952148</v>
@@ -3407,7 +3407,7 @@
         <v>-1.249875</v>
       </c>
       <c r="D58">
-        <v>-0.04166666666666667</v>
+        <v>0.04999500000000001</v>
       </c>
       <c r="E58">
         <v>-0.000275</v>
@@ -3424,7 +3424,7 @@
         <v>-33.16276775793094</v>
       </c>
       <c r="D59">
-        <v>-0.08586042281316755</v>
+        <v>2.622223999999996</v>
       </c>
       <c r="E59">
         <v>-0.002225838496404519</v>
@@ -3441,7 +3441,7 @@
         <v>-15.833664</v>
       </c>
       <c r="D60">
-        <v>-0.2307692307692307</v>
+        <v>2.968812</v>
       </c>
       <c r="E60">
         <v>-0.000704</v>
@@ -3458,7 +3458,7 @@
         <v>-115.3468481088867</v>
       </c>
       <c r="D61">
-        <v>-0.07552188145681991</v>
+        <v>8.099520000000012</v>
       </c>
       <c r="E61">
         <v>-0.01002580166092019</v>
@@ -3475,7 +3475,7 @@
         <v>-33.91925694396396</v>
       </c>
       <c r="D62">
-        <v>-0.07978991400873801</v>
+        <v>2.506426999999995</v>
       </c>
       <c r="E62">
         <v>-0.006401067549342132</v>
@@ -3492,7 +3492,7 @@
         <v>-0.884576</v>
       </c>
       <c r="D63">
-        <v>-1</v>
+        <v>0.442288</v>
       </c>
       <c r="E63">
         <v>-0.000176</v>
@@ -3509,7 +3509,7 @@
         <v>-4800.115915873123</v>
       </c>
       <c r="D64">
-        <v>-0.00126464429212268</v>
+        <v>6.062771944601991</v>
       </c>
       <c r="E64">
         <v>-0.2769191136421554</v>
@@ -3526,7 +3526,7 @@
         <v>-40.72940053258728</v>
       </c>
       <c r="D65">
-        <v>-0.0522592497073661</v>
+        <v>2.022778999999993</v>
       </c>
       <c r="E65">
         <v>-0.003765313907052536</v>
@@ -3543,7 +3543,7 @@
         <v>-49.18468434297895</v>
       </c>
       <c r="D66">
-        <v>-0.03039827447506027</v>
+        <v>1.451020999999997</v>
       </c>
       <c r="E66">
         <v>-0.00484721438286971</v>
@@ -3577,7 +3577,7 @@
         <v>-20.877483</v>
       </c>
       <c r="D68">
-        <v>-0.2965116279069768</v>
+        <v>4.774671000000001</v>
       </c>
       <c r="E68">
         <v>-0.002453</v>
@@ -3594,7 +3594,7 @@
         <v>-6.61881</v>
       </c>
       <c r="D69">
-        <v>-0.5499999999999999</v>
+        <v>2.34861</v>
       </c>
       <c r="E69">
         <v>-0.000682</v>
@@ -3611,7 +3611,7 @@
         <v>-56.16577232677464</v>
       </c>
       <c r="D70">
-        <v>-0.01568887616092797</v>
+        <v>0.8675666999999976</v>
       </c>
       <c r="E70">
         <v>-0.008331964445449435</v>
@@ -3628,7 +3628,7 @@
         <v>-117.6296698244545</v>
       </c>
       <c r="D71">
-        <v>-0.043569343613276</v>
+        <v>4.911075181600097</v>
       </c>
       <c r="E71">
         <v>-0.008056826700305105</v>
@@ -3645,7 +3645,7 @@
         <v>-5.379325069625706</v>
       </c>
       <c r="D72">
-        <v>-0.6396106976585841</v>
+        <v>2.09847</v>
       </c>
       <c r="E72">
         <v>-0.0008459388378087287</v>
@@ -3662,7 +3662,7 @@
         <v>-16.540832</v>
       </c>
       <c r="D73">
-        <v>-0.0148148148148147</v>
+        <v>0.2414719999999981</v>
       </c>
       <c r="E73">
         <v>-0.006028</v>
@@ -3679,7 +3679,7 @@
         <v>-64.80416053232467</v>
       </c>
       <c r="D74">
-        <v>-0.04609445167205013</v>
+        <v>2.855489999999996</v>
       </c>
       <c r="E74">
         <v>-0.002496404350411213</v>
@@ -3696,7 +3696,7 @@
         <v>-13.38424625928523</v>
       </c>
       <c r="D75">
-        <v>-0.1305816345475637</v>
+        <v>1.545874</v>
       </c>
       <c r="E75">
         <v>-0.002761916273067525</v>
@@ -3713,7 +3713,7 @@
         <v>-54.35309</v>
       </c>
       <c r="D76">
-        <v>-0.1521739130434783</v>
+        <v>7.178710000000002</v>
       </c>
       <c r="E76">
         <v>-0.00583</v>
@@ -3730,7 +3730,7 @@
         <v>-27.326706</v>
       </c>
       <c r="D77">
-        <v>-0.1201923076923077</v>
+        <v>2.93205</v>
       </c>
       <c r="E77">
         <v>-0.007689000000000001</v>
@@ -3747,7 +3747,7 @@
         <v>-13.540824</v>
       </c>
       <c r="D78">
-        <v>-0.1388888888888889</v>
+        <v>1.65132</v>
       </c>
       <c r="E78">
         <v>-0.002706</v>
@@ -3764,7 +3764,7 @@
         <v>-16.8399</v>
       </c>
       <c r="D79">
-        <v>-0.125</v>
+        <v>1.8711</v>
       </c>
       <c r="E79">
         <v>-0.000693</v>
@@ -3781,7 +3781,7 @@
         <v>-24.791338</v>
       </c>
       <c r="D80">
-        <v>-0.1275510204081632</v>
+        <v>2.804449999999999</v>
       </c>
       <c r="E80">
         <v>-0.002431</v>
@@ -3798,7 +3798,7 @@
         <v>-31.958311</v>
       </c>
       <c r="D81">
-        <v>-0.5265957446808511</v>
+        <v>11.023947</v>
       </c>
       <c r="E81">
         <v>-0.003157</v>
@@ -3815,7 +3815,7 @@
         <v>-39.511208</v>
       </c>
       <c r="D82">
-        <v>-0.03296703296703293</v>
+        <v>1.260995999999999</v>
       </c>
       <c r="E82">
         <v>-0.004136000000000001</v>
@@ -3832,7 +3832,7 @@
         <v>-12.796344</v>
       </c>
       <c r="D83">
-        <v>-0.7445652173913047</v>
+        <v>5.461368000000002</v>
       </c>
       <c r="E83">
         <v>-0.003531</v>
@@ -3849,7 +3849,7 @@
         <v>-7.506180000000001</v>
       </c>
       <c r="D84">
-        <v>-0.7983870967741936</v>
+        <v>3.33234</v>
       </c>
       <c r="E84">
         <v>-0.0004906</v>
@@ -3883,7 +3883,7 @@
         <v>-12.051831</v>
       </c>
       <c r="D86">
-        <v>-1.178571428571429</v>
+        <v>6.519843000000002</v>
       </c>
       <c r="E86">
         <v>-0.002013</v>
@@ -3900,7 +3900,7 @@
         <v>-21.89971229437467</v>
       </c>
       <c r="D87">
-        <v>-0.3161897013064567</v>
+        <v>5.260992000000005</v>
       </c>
       <c r="E87">
         <v>-0.002197883610435034</v>
@@ -3917,7 +3917,7 @@
         <v>-274.7811437071207</v>
       </c>
       <c r="D88">
-        <v>-0.1505068036906569</v>
+        <v>35.94627300000005</v>
       </c>
       <c r="E88">
         <v>-0.07172569660848883</v>
@@ -4049,7 +4049,7 @@
         <v>-22.936122</v>
       </c>
       <c r="D7">
-        <v>-0.3260869565217391</v>
+        <v>5.640029999999999</v>
       </c>
       <c r="E7">
         <v>-0.004026</v>
@@ -4066,7 +4066,7 @@
         <v>-35.58602305385697</v>
       </c>
       <c r="D8">
-        <v>-0.0906387451697976</v>
+        <v>2.957416000000002</v>
       </c>
       <c r="E8">
         <v>-0.001853052648086699</v>
@@ -4083,7 +4083,7 @@
         <v>-15.347728</v>
       </c>
       <c r="D9">
-        <v>-0.7058823529411766</v>
+        <v>6.350784000000001</v>
       </c>
       <c r="E9">
         <v>-0.001276</v>
@@ -4100,7 +4100,7 @@
         <v>-1628.910802378963</v>
       </c>
       <c r="D10">
-        <v>-0.02562377804797954</v>
+        <v>40.69606199999998</v>
       </c>
       <c r="E10">
         <v>-0.07308793477717784</v>
@@ -4117,7 +4117,7 @@
         <v>-61.73357873379457</v>
       </c>
       <c r="D11">
-        <v>-0.1639241068123903</v>
+        <v>8.694400000000002</v>
       </c>
       <c r="E11">
         <v>-0.02030709826769558</v>
@@ -4134,7 +4134,7 @@
         <v>-57.56036000000001</v>
       </c>
       <c r="D12">
-        <v>-0.1339869281045753</v>
+        <v>6.801080000000006</v>
       </c>
       <c r="E12">
         <v>-0.007634000000000001</v>
@@ -4151,7 +4151,7 @@
         <v>-4937.018531998421</v>
       </c>
       <c r="D13">
-        <v>-0.004643799278468943</v>
+        <v>22.82054904748111</v>
       </c>
       <c r="E13">
         <v>-1.782960827735074</v>
@@ -4168,7 +4168,7 @@
         <v>-118.0069566532047</v>
       </c>
       <c r="D14">
-        <v>-0.1079715878136511</v>
+        <v>11.499752</v>
       </c>
       <c r="E14">
         <v>-0.01535149689777608</v>
@@ -4185,7 +4185,7 @@
         <v>-86.24139232398362</v>
       </c>
       <c r="D15">
-        <v>-0.6590168918914264</v>
+        <v>34.25796</v>
       </c>
       <c r="E15">
         <v>-0.009082821729750777</v>
@@ -4202,7 +4202,7 @@
         <v>-78.992914</v>
       </c>
       <c r="D16">
-        <v>-1.077777777777778</v>
+        <v>40.974934</v>
       </c>
       <c r="E16">
         <v>-0.004114</v>
@@ -4219,7 +4219,7 @@
         <v>-102.2756062339354</v>
       </c>
       <c r="D17">
-        <v>-0.08047332407377961</v>
+        <v>7.617456000000004</v>
       </c>
       <c r="E17">
         <v>-0.007975327997031772</v>
@@ -4236,7 +4236,7 @@
         <v>-28.94377200000001</v>
       </c>
       <c r="D18">
-        <v>-0.3046875000000003</v>
+        <v>6.759324000000007</v>
       </c>
       <c r="E18">
         <v>-0.003674000000000001</v>
@@ -4253,7 +4253,7 @@
         <v>-77.53328683864774</v>
       </c>
       <c r="D19">
-        <v>-0.9630935116622715</v>
+        <v>38.037824</v>
       </c>
       <c r="E19">
         <v>-0.01273542819294477</v>
@@ -4270,7 +4270,7 @@
         <v>-44.293612</v>
       </c>
       <c r="D20">
-        <v>-0.4642857142857142</v>
+        <v>14.044316</v>
       </c>
       <c r="E20">
         <v>-0.001804</v>
@@ -4287,7 +4287,7 @@
         <v>-7.858224</v>
       </c>
       <c r="D21">
-        <v>-1.05</v>
+        <v>4.024944</v>
       </c>
       <c r="E21">
         <v>-0.000902</v>
@@ -4304,7 +4304,7 @@
         <v>-17.062078</v>
       </c>
       <c r="D22">
-        <v>-0.6562500000000001</v>
+        <v>6.760446000000002</v>
       </c>
       <c r="E22">
         <v>-0.001166</v>
@@ -4321,7 +4321,7 @@
         <v>-9.071062</v>
       </c>
       <c r="D23">
-        <v>-0.7499999999999997</v>
+        <v>3.887597999999999</v>
       </c>
       <c r="E23">
         <v>-0.002002</v>
@@ -4355,7 +4355,7 @@
         <v>-15.473524</v>
       </c>
       <c r="D25">
-        <v>-0.3387096774193549</v>
+        <v>3.914988000000001</v>
       </c>
       <c r="E25">
         <v>-0.001826</v>
@@ -4372,7 +4372,7 @@
         <v>-38.300152</v>
       </c>
       <c r="D26">
-        <v>-0.07971014492753625</v>
+        <v>2.827528000000001</v>
       </c>
       <c r="E26">
         <v>-0.003278000000000001</v>
@@ -4389,7 +4389,7 @@
         <v>-19.2885</v>
       </c>
       <c r="D27">
-        <v>-0.6025641025641025</v>
+        <v>7.252476</v>
       </c>
       <c r="E27">
         <v>-0.00275</v>
@@ -4406,7 +4406,7 @@
         <v>-12.820896</v>
       </c>
       <c r="D28">
-        <v>-0.3170731707317074</v>
+        <v>3.086512000000001</v>
       </c>
       <c r="E28">
         <v>-0.002376</v>
@@ -4423,7 +4423,7 @@
         <v>-839.0419260852415</v>
       </c>
       <c r="D29">
-        <v>-0.01594000690257538</v>
+        <v>13.164492</v>
       </c>
       <c r="E29">
         <v>-0.2537936860511922</v>
@@ -4440,7 +4440,7 @@
         <v>-29.21355895692437</v>
       </c>
       <c r="D30">
-        <v>-0.03552748740744487</v>
+        <v>1.002275999999995</v>
       </c>
       <c r="E30">
         <v>-0.001282477674916562</v>
@@ -4457,7 +4457,7 @@
         <v>-1324.24730488054</v>
       </c>
       <c r="D31">
-        <v>-0.03442195350865308</v>
+        <v>44.06633000000011</v>
       </c>
       <c r="E31">
         <v>-0.2505671343198751</v>
@@ -4474,7 +4474,7 @@
         <v>-49.42866913375786</v>
       </c>
       <c r="D32">
-        <v>-0.2260563503966258</v>
+        <v>9.113500000000002</v>
       </c>
       <c r="E32">
         <v>-0.002983021673733124</v>
@@ -4491,7 +4491,7 @@
         <v>-37.799916</v>
       </c>
       <c r="D33">
-        <v>-1.0625</v>
+        <v>19.47268399999999</v>
       </c>
       <c r="E33">
         <v>-0.001452</v>
@@ -4508,7 +4508,7 @@
         <v>-1581.717108601005</v>
       </c>
       <c r="D34">
-        <v>-0.008922966955548225</v>
+        <v>13.98878799999989</v>
       </c>
       <c r="E34">
         <v>-0.1442777623461649</v>
@@ -4525,7 +4525,7 @@
         <v>-86.58302400000001</v>
       </c>
       <c r="D35">
-        <v>-0.1750000000000001</v>
+        <v>12.89534400000001</v>
       </c>
       <c r="E35">
         <v>-0.002068</v>
@@ -4542,7 +4542,7 @@
         <v>-354.0806973800869</v>
       </c>
       <c r="D36">
-        <v>-0.01937903440528538</v>
+        <v>6.731295999999986</v>
       </c>
       <c r="E36">
         <v>-0.06017686903128601</v>
@@ -4559,7 +4559,7 @@
         <v>-2592.8933706367</v>
       </c>
       <c r="D37">
-        <v>-0.0003692193714174884</v>
+        <v>0.9569931200608153</v>
       </c>
       <c r="E37">
         <v>-2.611171571638167</v>
@@ -4576,7 +4576,7 @@
         <v>-5112.688629278012</v>
       </c>
       <c r="D38">
-        <v>-0.0001711868538888168</v>
+        <v>0.8750752799751353</v>
       </c>
       <c r="E38">
         <v>-5.630714349425123</v>
@@ -4593,7 +4593,7 @@
         <v>-4102.22917654558</v>
       </c>
       <c r="D39">
-        <v>-0.0002798806945988437</v>
+        <v>1.147813500495431</v>
       </c>
       <c r="E39">
         <v>-3.44435699122215</v>
@@ -4610,7 +4610,7 @@
         <v>-2120.068914812882</v>
       </c>
       <c r="D40">
-        <v>-0.0001650394940786302</v>
+        <v>0.3498373641309627</v>
       </c>
       <c r="E40">
         <v>-5.840410233644302</v>
@@ -4627,7 +4627,7 @@
         <v>-5844.279433095182</v>
       </c>
       <c r="D41">
-        <v>-9.399560167964729E-06</v>
+        <v>0.05493313982242398</v>
       </c>
       <c r="E41">
         <v>-102.5312181244769</v>
@@ -4644,7 +4644,7 @@
         <v>-3112.208591087726</v>
       </c>
       <c r="D42">
-        <v>-0.0007741397688689918</v>
+        <v>2.407420759226625</v>
       </c>
       <c r="E42">
         <v>-1.245880140547529</v>
@@ -4661,7 +4661,7 @@
         <v>-2588.122059432595</v>
       </c>
       <c r="D43">
-        <v>-0.000273394384562759</v>
+        <v>0.7073846426228556</v>
       </c>
       <c r="E43">
         <v>-3.526051852088004</v>
@@ -4678,7 +4678,7 @@
         <v>-304.827816355602</v>
       </c>
       <c r="D44">
-        <v>-0.04415328514276378</v>
+        <v>12.89001307231888</v>
       </c>
       <c r="E44">
         <v>-0.02279086477425062</v>
@@ -4695,7 +4695,7 @@
         <v>-11.16819917126869</v>
       </c>
       <c r="D45">
-        <v>-0.1124080559759308</v>
+        <v>1.128538714593306</v>
       </c>
       <c r="E45">
         <v>-0.009537317823457465</v>
@@ -4712,7 +4712,7 @@
         <v>-1445.487049268444</v>
       </c>
       <c r="D46">
-        <v>-0.0008548020776936675</v>
+        <v>1.234550037057261</v>
       </c>
       <c r="E46">
         <v>-1.128405190685748</v>
@@ -4729,7 +4729,7 @@
         <v>-3659.052304446318</v>
       </c>
       <c r="D47">
-        <v>-0.001793702473606149</v>
+        <v>6.55149972827121</v>
       </c>
       <c r="E47">
         <v>-0.5382542371942215</v>
@@ -4746,7 +4746,7 @@
         <v>-5015.248641768412</v>
       </c>
       <c r="D48">
-        <v>-0.0004992934100192883</v>
+        <v>2.502830949443705</v>
       </c>
       <c r="E48">
         <v>-1.931170058439897</v>
@@ -4763,7 +4763,7 @@
         <v>-3312.496976082596</v>
       </c>
       <c r="D49">
-        <v>-0.0005516362499345261</v>
+        <v>1.826285964265026</v>
       </c>
       <c r="E49">
         <v>-1.748019512444642</v>
@@ -4780,7 +4780,7 @@
         <v>-63016.31375774965</v>
       </c>
       <c r="D50">
-        <v>-1.1669068198079E-05</v>
+        <v>0.7353330821788404</v>
       </c>
       <c r="E50">
         <v>-82.5901884112053</v>
@@ -4797,7 +4797,7 @@
         <v>-5029.585174395654</v>
       </c>
       <c r="D51">
-        <v>-0.0002852030565469383</v>
+        <v>1.434044071148492</v>
       </c>
       <c r="E51">
         <v>-3.380097563437939</v>
@@ -4814,7 +4814,7 @@
         <v>-191.3765697272249</v>
       </c>
       <c r="D52">
-        <v>-0.02518338804373868</v>
+        <v>4.701120281627794</v>
       </c>
       <c r="E52">
         <v>-0.0392325891199723</v>
@@ -4831,7 +4831,7 @@
         <v>-8351.287885486006</v>
       </c>
       <c r="D53">
-        <v>-0.0001834043590695663</v>
+        <v>1.531381739956487</v>
       </c>
       <c r="E53">
         <v>-5.255687781929519</v>
@@ -4848,7 +4848,7 @@
         <v>-46.9953</v>
       </c>
       <c r="D54">
-        <v>-0.07142857142857148</v>
+        <v>3.133020000000002</v>
       </c>
       <c r="E54">
         <v>-0.00198</v>
@@ -4882,7 +4882,7 @@
         <v>-47.40030471060579</v>
       </c>
       <c r="D56">
-        <v>-0.005561354973102513</v>
+        <v>0.2621519999999933</v>
       </c>
       <c r="E56">
         <v>-0.003977870485952148</v>
@@ -4916,7 +4916,7 @@
         <v>-1.29987</v>
       </c>
       <c r="D58">
-        <v>-0.08333333333333316</v>
+        <v>0.0999899999999998</v>
       </c>
       <c r="E58">
         <v>-0.000286</v>
@@ -4933,7 +4933,7 @@
         <v>-35.78499175793094</v>
       </c>
       <c r="D59">
-        <v>-0.1717208456263353</v>
+        <v>5.244447999999998</v>
       </c>
       <c r="E59">
         <v>-0.00240183849640452</v>
@@ -4950,7 +4950,7 @@
         <v>-18.802476</v>
       </c>
       <c r="D60">
-        <v>-0.4615384615384616</v>
+        <v>5.937624000000001</v>
       </c>
       <c r="E60">
         <v>-0.000836</v>
@@ -4967,7 +4967,7 @@
         <v>-123.4463681088867</v>
       </c>
       <c r="D61">
-        <v>-0.1510437629136396</v>
+        <v>16.19904</v>
       </c>
       <c r="E61">
         <v>-0.01072980166092018</v>
@@ -4984,7 +4984,7 @@
         <v>-36.42568394396396</v>
       </c>
       <c r="D62">
-        <v>-0.1595798280174762</v>
+        <v>5.012853999999997</v>
       </c>
       <c r="E62">
         <v>-0.006874067549342133</v>
@@ -5001,7 +5001,7 @@
         <v>-1.326864</v>
       </c>
       <c r="D63">
-        <v>-2</v>
+        <v>0.8845760000000003</v>
       </c>
       <c r="E63">
         <v>-0.0002640000000000001</v>
@@ -5018,7 +5018,7 @@
         <v>-4816.704553873123</v>
       </c>
       <c r="D64">
-        <v>-0.004724897547973427</v>
+        <v>22.65140994460216</v>
       </c>
       <c r="E64">
         <v>-0.2778761136421555</v>
@@ -5035,7 +5035,7 @@
         <v>-42.75217953258729</v>
       </c>
       <c r="D65">
-        <v>-0.1045184994147326</v>
+        <v>4.045558</v>
       </c>
       <c r="E65">
         <v>-0.003952313907052537</v>
@@ -5052,7 +5052,7 @@
         <v>-50.63570534297894</v>
       </c>
       <c r="D66">
-        <v>-0.06079654895012054</v>
+        <v>2.902041999999994</v>
       </c>
       <c r="E66">
         <v>-0.00499021438286971</v>
@@ -5086,7 +5086,7 @@
         <v>-25.652154</v>
       </c>
       <c r="D68">
-        <v>-0.5930232558139534</v>
+        <v>9.549341999999999</v>
       </c>
       <c r="E68">
         <v>-0.003014</v>
@@ -5103,7 +5103,7 @@
         <v>-8.967420000000001</v>
       </c>
       <c r="D69">
-        <v>-1.1</v>
+        <v>4.697220000000001</v>
       </c>
       <c r="E69">
         <v>-0.000924</v>
@@ -5120,7 +5120,7 @@
         <v>-57.03333902677464</v>
       </c>
       <c r="D70">
-        <v>-0.03137775232185594</v>
+        <v>1.735133399999995</v>
       </c>
       <c r="E70">
         <v>-0.008460664445449436</v>
@@ -5137,7 +5137,7 @@
         <v>-127.5868698244545</v>
       </c>
       <c r="D71">
-        <v>-0.1319061440457963</v>
+        <v>14.86827518160008</v>
       </c>
       <c r="E71">
         <v>-0.008738826700305104</v>
@@ -5154,7 +5154,7 @@
         <v>-7.477795069625705</v>
       </c>
       <c r="D72">
-        <v>-1.279221395317168</v>
+        <v>4.19694</v>
       </c>
       <c r="E72">
         <v>-0.001175938837808728</v>
@@ -5171,7 +5171,7 @@
         <v>-16.782304</v>
       </c>
       <c r="D73">
-        <v>-0.02962962962962962</v>
+        <v>0.4829439999999998</v>
       </c>
       <c r="E73">
         <v>-0.006116</v>
@@ -5188,7 +5188,7 @@
         <v>-67.65965053232468</v>
       </c>
       <c r="D74">
-        <v>-0.09218890334410039</v>
+        <v>5.710979999999999</v>
       </c>
       <c r="E74">
         <v>-0.002606404350411213</v>
@@ -5205,7 +5205,7 @@
         <v>-14.93012025928523</v>
       </c>
       <c r="D75">
-        <v>-0.2611632690951275</v>
+        <v>3.091748000000001</v>
       </c>
       <c r="E75">
         <v>-0.003080916273067526</v>
@@ -5222,7 +5222,7 @@
         <v>-61.5318</v>
       </c>
       <c r="D76">
-        <v>-0.3043478260869567</v>
+        <v>14.35742</v>
       </c>
       <c r="E76">
         <v>-0.006600000000000001</v>
@@ -5239,7 +5239,7 @@
         <v>-30.25875600000001</v>
       </c>
       <c r="D77">
-        <v>-0.2403846153846155</v>
+        <v>5.864100000000004</v>
       </c>
       <c r="E77">
         <v>-0.008514000000000001</v>
@@ -5256,7 +5256,7 @@
         <v>-15.192144</v>
       </c>
       <c r="D78">
-        <v>-0.2777777777777778</v>
+        <v>3.30264</v>
       </c>
       <c r="E78">
         <v>-0.003036</v>
@@ -5273,7 +5273,7 @@
         <v>-18.711</v>
       </c>
       <c r="D79">
-        <v>-0.2500000000000002</v>
+        <v>3.742200000000002</v>
       </c>
       <c r="E79">
         <v>-0.0007700000000000001</v>
@@ -5290,7 +5290,7 @@
         <v>-27.595788</v>
       </c>
       <c r="D80">
-        <v>-0.2551020408163264</v>
+        <v>5.608899999999998</v>
       </c>
       <c r="E80">
         <v>-0.002706</v>
@@ -5307,7 +5307,7 @@
         <v>-42.98225799999999</v>
       </c>
       <c r="D81">
-        <v>-1.053191489361702</v>
+        <v>22.047894</v>
       </c>
       <c r="E81">
         <v>-0.004246</v>
@@ -5324,7 +5324,7 @@
         <v>-40.772204</v>
       </c>
       <c r="D82">
-        <v>-0.06593406593406567</v>
+        <v>2.52199199999999</v>
       </c>
       <c r="E82">
         <v>-0.004267999999999999</v>
@@ -5341,7 +5341,7 @@
         <v>-18.257712</v>
       </c>
       <c r="D83">
-        <v>-1.489130434782609</v>
+        <v>10.922736</v>
       </c>
       <c r="E83">
         <v>-0.005037999999999999</v>
@@ -5358,7 +5358,7 @@
         <v>-10.83852</v>
       </c>
       <c r="D84">
-        <v>-1.596774193548387</v>
+        <v>6.664679999999999</v>
       </c>
       <c r="E84">
         <v>-0.0007084</v>
@@ -5375,7 +5375,7 @@
         <v>-26.00274515598377</v>
       </c>
       <c r="D85">
-        <v>-0.1798051753829248</v>
+        <v>3.962881542447612</v>
       </c>
       <c r="E85">
         <v>-0.001542365807935451</v>
@@ -5392,7 +5392,7 @@
         <v>-18.571674</v>
       </c>
       <c r="D86">
-        <v>-2.357142857142857</v>
+        <v>13.039686</v>
       </c>
       <c r="E86">
         <v>-0.003102</v>
@@ -5409,7 +5409,7 @@
         <v>-27.16070429437467</v>
       </c>
       <c r="D87">
-        <v>-0.6323794026129127</v>
+        <v>10.521984</v>
       </c>
       <c r="E87">
         <v>-0.002725883610435033</v>
@@ -5426,7 +5426,7 @@
         <v>-310.7274167071207</v>
       </c>
       <c r="D88">
-        <v>-0.3010136073813136</v>
+        <v>71.89254600000001</v>
       </c>
       <c r="E88">
         <v>-0.08110869660848884</v>
@@ -5558,7 +5558,7 @@
         <v>-25.756137</v>
       </c>
       <c r="D7">
-        <v>-0.4891304347826087</v>
+        <v>8.460045000000001</v>
       </c>
       <c r="E7">
         <v>-0.004521000000000001</v>
@@ -5575,7 +5575,7 @@
         <v>-37.06473105385697</v>
       </c>
       <c r="D8">
-        <v>-0.1359581177546965</v>
+        <v>4.436124000000007</v>
       </c>
       <c r="E8">
         <v>-0.001930052648086699</v>
@@ -5592,7 +5592,7 @@
         <v>-18.52312</v>
       </c>
       <c r="D9">
-        <v>-1.058823529411765</v>
+        <v>9.526176</v>
       </c>
       <c r="E9">
         <v>-0.00154</v>
@@ -5609,7 +5609,7 @@
         <v>-1649.258833378963</v>
       </c>
       <c r="D10">
-        <v>-0.03843566707196931</v>
+        <v>61.04409299999998</v>
       </c>
       <c r="E10">
         <v>-0.07400093477717784</v>
@@ -5626,7 +5626,7 @@
         <v>-66.08077873379457</v>
       </c>
       <c r="D11">
-        <v>-0.2458861602185854</v>
+        <v>13.0416</v>
       </c>
       <c r="E11">
         <v>-0.02173709826769558</v>
@@ -5643,7 +5643,7 @@
         <v>-60.9609</v>
       </c>
       <c r="D12">
-        <v>-0.2009803921568627</v>
+        <v>10.20162</v>
       </c>
       <c r="E12">
         <v>-0.008085</v>
@@ -5660,7 +5660,7 @@
         <v>-4949.872229998421</v>
       </c>
       <c r="D13">
-        <v>-0.007259424054799453</v>
+        <v>35.674247047481</v>
       </c>
       <c r="E13">
         <v>-1.787602827735074</v>
@@ -5677,7 +5677,7 @@
         <v>-123.7568326532047</v>
       </c>
       <c r="D14">
-        <v>-0.1619573817204764</v>
+        <v>17.24962799999997</v>
       </c>
       <c r="E14">
         <v>-0.01609949689777608</v>
@@ -5694,7 +5694,7 @@
         <v>-103.3703723239836</v>
       </c>
       <c r="D15">
-        <v>-0.9885253378371397</v>
+        <v>51.38694</v>
       </c>
       <c r="E15">
         <v>-0.01088682172975078</v>
@@ -5711,7 +5711,7 @@
         <v>-99.48038099999999</v>
       </c>
       <c r="D16">
-        <v>-1.616666666666666</v>
+        <v>61.46240099999999</v>
       </c>
       <c r="E16">
         <v>-0.005181</v>
@@ -5728,7 +5728,7 @@
         <v>-106.0843342339354</v>
       </c>
       <c r="D17">
-        <v>-0.1207099861106693</v>
+        <v>11.42618399999999</v>
       </c>
       <c r="E17">
         <v>-0.008272327997031771</v>
@@ -5745,7 +5745,7 @@
         <v>-32.32343400000001</v>
       </c>
       <c r="D18">
-        <v>-0.4570312500000001</v>
+        <v>10.138986</v>
       </c>
       <c r="E18">
         <v>-0.004103000000000001</v>
@@ -5762,7 +5762,7 @@
         <v>-96.55219883864774</v>
       </c>
       <c r="D19">
-        <v>-1.444640267493407</v>
+        <v>57.056736</v>
       </c>
       <c r="E19">
         <v>-0.01585942819294477</v>
@@ -5779,7 +5779,7 @@
         <v>-51.31577</v>
       </c>
       <c r="D20">
-        <v>-0.6964285714285716</v>
+        <v>21.066474</v>
       </c>
       <c r="E20">
         <v>-0.00209</v>
@@ -5796,7 +5796,7 @@
         <v>-9.870696000000001</v>
       </c>
       <c r="D21">
-        <v>-1.575</v>
+        <v>6.037416</v>
       </c>
       <c r="E21">
         <v>-0.001133</v>
@@ -5813,7 +5813,7 @@
         <v>-20.442301</v>
       </c>
       <c r="D22">
-        <v>-0.9843749999999998</v>
+        <v>10.140669</v>
       </c>
       <c r="E22">
         <v>-0.001397</v>
@@ -5830,7 +5830,7 @@
         <v>-11.014861</v>
       </c>
       <c r="D23">
-        <v>-1.125</v>
+        <v>5.831397000000001</v>
       </c>
       <c r="E23">
         <v>-0.002431</v>
@@ -5864,7 +5864,7 @@
         <v>-17.431018</v>
       </c>
       <c r="D25">
-        <v>-0.5080645161290321</v>
+        <v>5.872482</v>
       </c>
       <c r="E25">
         <v>-0.002057</v>
@@ -5881,7 +5881,7 @@
         <v>-39.713916</v>
       </c>
       <c r="D26">
-        <v>-0.1195652173913042</v>
+        <v>4.241291999999994</v>
       </c>
       <c r="E26">
         <v>-0.003399</v>
@@ -5898,7 +5898,7 @@
         <v>-22.914738</v>
       </c>
       <c r="D27">
-        <v>-0.9038461538461536</v>
+        <v>10.878714</v>
       </c>
       <c r="E27">
         <v>-0.003267</v>
@@ -5915,7 +5915,7 @@
         <v>-14.364152</v>
       </c>
       <c r="D28">
-        <v>-0.475609756097561</v>
+        <v>4.629768</v>
       </c>
       <c r="E28">
         <v>-0.002662</v>
@@ -5932,7 +5932,7 @@
         <v>-845.6241720852414</v>
       </c>
       <c r="D29">
-        <v>-0.02391001035386301</v>
+        <v>19.74673799999994</v>
       </c>
       <c r="E29">
         <v>-0.2557846860511922</v>
@@ -5949,7 +5949,7 @@
         <v>-29.71469695692438</v>
       </c>
       <c r="D30">
-        <v>-0.05329123111116768</v>
+        <v>1.503414000000003</v>
       </c>
       <c r="E30">
         <v>-0.001304477674916563</v>
@@ -5966,7 +5966,7 @@
         <v>-1346.28046988054</v>
       </c>
       <c r="D31">
-        <v>-0.05163293026297944</v>
+        <v>66.09949499999993</v>
       </c>
       <c r="E31">
         <v>-0.254736134319875</v>
@@ -5983,7 +5983,7 @@
         <v>-53.98541913375786</v>
       </c>
       <c r="D32">
-        <v>-0.3390845255949386</v>
+        <v>13.67025</v>
       </c>
       <c r="E32">
         <v>-0.003258021673733124</v>
@@ -6000,7 +6000,7 @@
         <v>-47.536258</v>
       </c>
       <c r="D33">
-        <v>-1.59375</v>
+        <v>29.209026</v>
       </c>
       <c r="E33">
         <v>-0.001826</v>
@@ -6017,7 +6017,7 @@
         <v>-1588.711502601005</v>
       </c>
       <c r="D34">
-        <v>-0.01338445043332241</v>
+        <v>20.98318199999994</v>
       </c>
       <c r="E34">
         <v>-0.1449157623461649</v>
@@ -6034,7 +6034,7 @@
         <v>-93.03069600000002</v>
       </c>
       <c r="D35">
-        <v>-0.2625000000000003</v>
+        <v>19.34301600000002</v>
       </c>
       <c r="E35">
         <v>-0.002222</v>
@@ -6051,7 +6051,7 @@
         <v>-357.4463453800869</v>
       </c>
       <c r="D36">
-        <v>-0.02906855160792816</v>
+        <v>10.09694400000001</v>
       </c>
       <c r="E36">
         <v>-0.06074886903128601</v>
@@ -6068,7 +6068,7 @@
         <v>-2593.37186719673</v>
       </c>
       <c r="D37">
-        <v>-0.0005538290571261449</v>
+        <v>1.435489680090996</v>
       </c>
       <c r="E37">
         <v>-2.61165344128573</v>
@@ -6085,7 +6085,7 @@
         <v>-5113.126166917999</v>
       </c>
       <c r="D38">
-        <v>-0.0002567802808332252</v>
+        <v>1.312612919962703</v>
       </c>
       <c r="E38">
         <v>-5.631196219072686</v>
@@ -6102,7 +6102,7 @@
         <v>-4102.803083295828</v>
       </c>
       <c r="D39">
-        <v>-0.0004198210418983764</v>
+        <v>1.721720250743601</v>
       </c>
       <c r="E39">
         <v>-3.444838860869713</v>
@@ -6119,7 +6119,7 @@
         <v>-2120.243833494947</v>
       </c>
       <c r="D40">
-        <v>-0.0002475592411180526</v>
+        <v>0.5247560461966714</v>
       </c>
       <c r="E40">
         <v>-5.840892103291866</v>
@@ -6136,7 +6136,7 @@
         <v>-5844.306899665093</v>
       </c>
       <c r="D41">
-        <v>-1.409934025186928E-05</v>
+        <v>0.08239970973318123</v>
       </c>
       <c r="E41">
         <v>-102.5316999941244</v>
@@ -6153,7 +6153,7 @@
         <v>-3113.412301467339</v>
       </c>
       <c r="D42">
-        <v>-0.001161209653303341</v>
+        <v>3.611131138839482</v>
       </c>
       <c r="E42">
         <v>-1.246362010195092</v>
@@ -6170,7 +6170,7 @@
         <v>-2588.475751753906</v>
       </c>
       <c r="D43">
-        <v>-0.0004100915768441386</v>
+        <v>1.061076963934283</v>
       </c>
       <c r="E43">
         <v>-3.526533721735567</v>
@@ -6187,7 +6187,7 @@
         <v>-311.2728228917615</v>
       </c>
       <c r="D44">
-        <v>-0.06622992771414586</v>
+        <v>19.33501960847838</v>
       </c>
       <c r="E44">
         <v>-0.02327273442181394</v>
@@ -6204,7 +6204,7 @@
         <v>-11.73246852856534</v>
       </c>
       <c r="D45">
-        <v>-0.1686120839638962</v>
+        <v>1.692808071889958</v>
       </c>
       <c r="E45">
         <v>-0.01001918747102079</v>
@@ -6221,7 +6221,7 @@
         <v>-1446.104324286972</v>
       </c>
       <c r="D46">
-        <v>-0.001282203116540422</v>
+        <v>1.851825055585778</v>
       </c>
       <c r="E46">
         <v>-1.128887060333312</v>
@@ -6238,7 +6238,7 @@
         <v>-3662.328054310453</v>
       </c>
       <c r="D47">
-        <v>-0.002690553710409161</v>
+        <v>9.827249592406588</v>
       </c>
       <c r="E47">
         <v>-0.5387361068417849</v>
@@ -6255,7 +6255,7 @@
         <v>-5016.500057243135</v>
       </c>
       <c r="D48">
-        <v>-0.0007489401150290232</v>
+        <v>3.754246424166013</v>
       </c>
       <c r="E48">
         <v>-1.93165192808746</v>
@@ -6272,7 +6272,7 @@
         <v>-3313.410119064729</v>
       </c>
       <c r="D49">
-        <v>-0.0008274543749018578</v>
+        <v>2.739428946397766</v>
       </c>
       <c r="E49">
         <v>-1.748501382092205</v>
@@ -6289,7 +6289,7 @@
         <v>-63016.68142429073</v>
       </c>
       <c r="D50">
-        <v>-1.75036022971185E-05</v>
+        <v>1.102999623268261</v>
       </c>
       <c r="E50">
         <v>-82.59067028085286</v>
@@ -6306,7 +6306,7 @@
         <v>-5030.302196431228</v>
       </c>
       <c r="D51">
-        <v>-0.0004278045848204979</v>
+        <v>2.151066106723192</v>
       </c>
       <c r="E51">
         <v>-3.380579433085503</v>
@@ -6323,7 +6323,7 @@
         <v>-193.7271298680388</v>
       </c>
       <c r="D52">
-        <v>-0.03777508206560794</v>
+        <v>7.051680422441677</v>
       </c>
       <c r="E52">
         <v>-0.03971445876753562</v>
@@ -6340,7 +6340,7 @@
         <v>-8352.053576355984</v>
       </c>
       <c r="D53">
-        <v>-0.0002751065386042405</v>
+        <v>2.297072609933821</v>
       </c>
       <c r="E53">
         <v>-5.256169651577082</v>
@@ -6357,7 +6357,7 @@
         <v>-48.56181000000001</v>
       </c>
       <c r="D54">
-        <v>-0.1071428571428574</v>
+        <v>4.69953000000001</v>
       </c>
       <c r="E54">
         <v>-0.002046000000000001</v>
@@ -6391,7 +6391,7 @@
         <v>-47.5313807106058</v>
       </c>
       <c r="D56">
-        <v>-0.008342032459653845</v>
+        <v>0.3932279999999935</v>
       </c>
       <c r="E56">
         <v>-0.003988870485952148</v>
@@ -6425,7 +6425,7 @@
         <v>-1.349865</v>
       </c>
       <c r="D58">
-        <v>-0.1249999999999998</v>
+        <v>0.1499849999999998</v>
       </c>
       <c r="E58">
         <v>-0.000297</v>
@@ -6442,7 +6442,7 @@
         <v>-38.40721575793094</v>
       </c>
       <c r="D59">
-        <v>-0.2575812684395031</v>
+        <v>7.866672000000001</v>
       </c>
       <c r="E59">
         <v>-0.00257783849640452</v>
@@ -6459,7 +6459,7 @@
         <v>-21.771288</v>
       </c>
       <c r="D60">
-        <v>-0.6923076923076924</v>
+        <v>8.906436000000001</v>
       </c>
       <c r="E60">
         <v>-0.0009680000000000001</v>
@@ -6476,7 +6476,7 @@
         <v>-131.5458881088867</v>
       </c>
       <c r="D61">
-        <v>-0.2265656443704591</v>
+        <v>24.29855999999997</v>
       </c>
       <c r="E61">
         <v>-0.01143380166092018</v>
@@ -6493,7 +6493,7 @@
         <v>-38.93211094396396</v>
       </c>
       <c r="D62">
-        <v>-0.2393697420262145</v>
+        <v>7.519280999999999</v>
       </c>
       <c r="E62">
         <v>-0.007347067549342133</v>
@@ -6510,7 +6510,7 @@
         <v>-1.769152</v>
       </c>
       <c r="D63">
-        <v>-3</v>
+        <v>1.326864</v>
       </c>
       <c r="E63">
         <v>-0.000352</v>
@@ -6527,7 +6527,7 @@
         <v>-4833.293191873122</v>
       </c>
       <c r="D64">
-        <v>-0.008185150803823983</v>
+        <v>39.24004794460143</v>
       </c>
       <c r="E64">
         <v>-0.2788331136421554</v>
@@ -6544,7 +6544,7 @@
         <v>-44.77495853258728</v>
       </c>
       <c r="D65">
-        <v>-0.1567777491220987</v>
+        <v>6.068336999999993</v>
       </c>
       <c r="E65">
         <v>-0.004139313907052536</v>
@@ -6561,7 +6561,7 @@
         <v>-52.08672634297895</v>
       </c>
       <c r="D66">
-        <v>-0.09119482342518097</v>
+        <v>4.353062999999999</v>
       </c>
       <c r="E66">
         <v>-0.00513321438286971</v>
@@ -6595,7 +6595,7 @@
         <v>-30.426825</v>
       </c>
       <c r="D68">
-        <v>-0.8895348837209303</v>
+        <v>14.324013</v>
       </c>
       <c r="E68">
         <v>-0.003575</v>
@@ -6612,7 +6612,7 @@
         <v>-11.31603</v>
       </c>
       <c r="D69">
-        <v>-1.65</v>
+        <v>7.045830000000001</v>
       </c>
       <c r="E69">
         <v>-0.001166</v>
@@ -6629,7 +6629,7 @@
         <v>-57.90090572677465</v>
       </c>
       <c r="D70">
-        <v>-0.04706662848278416</v>
+        <v>2.602700100000007</v>
       </c>
       <c r="E70">
         <v>-0.008589364445449436</v>
@@ -6646,7 +6646,7 @@
         <v>-137.5440698244545</v>
       </c>
       <c r="D71">
-        <v>-0.2202429444783169</v>
+        <v>24.8254751816001</v>
       </c>
       <c r="E71">
         <v>-0.009420826700305106</v>
@@ -6663,7 +6663,7 @@
         <v>-9.576265069625704</v>
       </c>
       <c r="D72">
-        <v>-1.918832092975752</v>
+        <v>6.295409999999999</v>
       </c>
       <c r="E72">
         <v>-0.001505938837808728</v>
@@ -6680,7 +6680,7 @@
         <v>-17.023776</v>
       </c>
       <c r="D73">
-        <v>-0.04444444444444454</v>
+        <v>0.7244160000000015</v>
       </c>
       <c r="E73">
         <v>-0.006204</v>
@@ -6697,7 +6697,7 @@
         <v>-70.51514053232468</v>
       </c>
       <c r="D74">
-        <v>-0.1382833550161506</v>
+        <v>8.566470000000002</v>
       </c>
       <c r="E74">
         <v>-0.002716404350411213</v>
@@ -6714,7 +6714,7 @@
         <v>-16.47599425928523</v>
       </c>
       <c r="D75">
-        <v>-0.3917449036426914</v>
+        <v>4.637622000000002</v>
       </c>
       <c r="E75">
         <v>-0.003399916273067526</v>
@@ -6731,7 +6731,7 @@
         <v>-68.71051</v>
       </c>
       <c r="D76">
-        <v>-0.4565217391304348</v>
+        <v>21.53613</v>
       </c>
       <c r="E76">
         <v>-0.00737</v>
@@ -6748,7 +6748,7 @@
         <v>-33.190806</v>
       </c>
       <c r="D77">
-        <v>-0.3605769230769231</v>
+        <v>8.796150000000001</v>
       </c>
       <c r="E77">
         <v>-0.009339</v>
@@ -6765,7 +6765,7 @@
         <v>-16.843464</v>
       </c>
       <c r="D78">
-        <v>-0.4166666666666667</v>
+        <v>4.95396</v>
       </c>
       <c r="E78">
         <v>-0.003366</v>
@@ -6782,7 +6782,7 @@
         <v>-20.5821</v>
       </c>
       <c r="D79">
-        <v>-0.3750000000000001</v>
+        <v>5.613300000000001</v>
       </c>
       <c r="E79">
         <v>-0.000847</v>
@@ -6799,7 +6799,7 @@
         <v>-30.400238</v>
       </c>
       <c r="D80">
-        <v>-0.3826530612244894</v>
+        <v>8.413349999999994</v>
       </c>
       <c r="E80">
         <v>-0.002981</v>
@@ -6816,7 +6816,7 @@
         <v>-54.006205</v>
       </c>
       <c r="D81">
-        <v>-1.579787234042554</v>
+        <v>33.07184100000001</v>
       </c>
       <c r="E81">
         <v>-0.005335</v>
@@ -6833,7 +6833,7 @@
         <v>-42.0332</v>
       </c>
       <c r="D82">
-        <v>-0.09890109890109879</v>
+        <v>3.782987999999996</v>
       </c>
       <c r="E82">
         <v>-0.0044</v>
@@ -6850,7 +6850,7 @@
         <v>-23.71908</v>
       </c>
       <c r="D83">
-        <v>-2.233695652173914</v>
+        <v>16.384104</v>
       </c>
       <c r="E83">
         <v>-0.006545</v>
@@ -6867,7 +6867,7 @@
         <v>-14.17086</v>
       </c>
       <c r="D84">
-        <v>-2.395161290322581</v>
+        <v>9.997020000000001</v>
       </c>
       <c r="E84">
         <v>-0.0009262000000000001</v>
@@ -6884,7 +6884,7 @@
         <v>-30.63897015598377</v>
       </c>
       <c r="D85">
-        <v>-0.3901615133936819</v>
+        <v>8.599106542447611</v>
       </c>
       <c r="E85">
         <v>-0.001817365807935451</v>
@@ -6901,7 +6901,7 @@
         <v>-25.091517</v>
       </c>
       <c r="D86">
-        <v>-3.535714285714286</v>
+        <v>19.559529</v>
       </c>
       <c r="E86">
         <v>-0.004191</v>
@@ -6918,7 +6918,7 @@
         <v>-32.42169629437468</v>
       </c>
       <c r="D87">
-        <v>-0.9485691039193697</v>
+        <v>15.78297600000001</v>
       </c>
       <c r="E87">
         <v>-0.003253883610435034</v>
@@ -6935,7 +6935,7 @@
         <v>-346.6736897071207</v>
       </c>
       <c r="D88">
-        <v>-0.4515204110719703</v>
+        <v>107.838819</v>
       </c>
       <c r="E88">
         <v>-0.09049169660848884</v>
@@ -7067,7 +7067,7 @@
         <v>-28.576152</v>
       </c>
       <c r="D7">
-        <v>-0.6521739130434784</v>
+        <v>11.28006</v>
       </c>
       <c r="E7">
         <v>-0.005016</v>
@@ -7084,7 +7084,7 @@
         <v>-38.54343905385697</v>
       </c>
       <c r="D8">
-        <v>-0.1812774903395952</v>
+        <v>5.914832000000004</v>
       </c>
       <c r="E8">
         <v>-0.002007052648086699</v>
@@ -7101,7 +7101,7 @@
         <v>-21.698512</v>
       </c>
       <c r="D9">
-        <v>-1.411764705882353</v>
+        <v>12.701568</v>
       </c>
       <c r="E9">
         <v>-0.001804</v>
@@ -7118,7 +7118,7 @@
         <v>-1669.606864378963</v>
       </c>
       <c r="D10">
-        <v>-0.05124755609595907</v>
+        <v>81.39212399999997</v>
       </c>
       <c r="E10">
         <v>-0.07491393477717785</v>
@@ -7135,7 +7135,7 @@
         <v>-70.42797873379457</v>
       </c>
       <c r="D11">
-        <v>-0.3278482136247806</v>
+        <v>17.3888</v>
       </c>
       <c r="E11">
         <v>-0.02316709826769559</v>
@@ -7152,7 +7152,7 @@
         <v>-64.36144</v>
       </c>
       <c r="D12">
-        <v>-0.2679738562091503</v>
+        <v>13.60216</v>
       </c>
       <c r="E12">
         <v>-0.008536</v>
@@ -7169,7 +7169,7 @@
         <v>-4962.725927998421</v>
       </c>
       <c r="D13">
-        <v>-0.009875048831129963</v>
+        <v>48.5279450474809</v>
       </c>
       <c r="E13">
         <v>-1.792244827735074</v>
@@ -7186,7 +7186,7 @@
         <v>-129.5067086532047</v>
       </c>
       <c r="D14">
-        <v>-0.2159431756273019</v>
+        <v>22.99950399999997</v>
       </c>
       <c r="E14">
         <v>-0.01684749689777608</v>
@@ -7203,7 +7203,7 @@
         <v>-120.4993523239836</v>
       </c>
       <c r="D15">
-        <v>-1.318033783782853</v>
+        <v>68.51591999999999</v>
       </c>
       <c r="E15">
         <v>-0.01269082172975078</v>
@@ -7220,7 +7220,7 @@
         <v>-119.967848</v>
       </c>
       <c r="D16">
-        <v>-2.155555555555556</v>
+        <v>81.94986800000001</v>
       </c>
       <c r="E16">
         <v>-0.006248</v>
@@ -7237,7 +7237,7 @@
         <v>-109.8930622339354</v>
       </c>
       <c r="D17">
-        <v>-0.1609466481475591</v>
+        <v>15.23491199999999</v>
       </c>
       <c r="E17">
         <v>-0.008569327997031771</v>
@@ -7254,7 +7254,7 @@
         <v>-35.703096</v>
       </c>
       <c r="D18">
-        <v>-0.6093749999999999</v>
+        <v>13.518648</v>
       </c>
       <c r="E18">
         <v>-0.004532</v>
@@ -7271,7 +7271,7 @@
         <v>-115.5711108386477</v>
       </c>
       <c r="D19">
-        <v>-1.926187023324543</v>
+        <v>76.075648</v>
       </c>
       <c r="E19">
         <v>-0.01898342819294477</v>
@@ -7288,7 +7288,7 @@
         <v>-58.33792800000001</v>
       </c>
       <c r="D20">
-        <v>-0.9285714285714289</v>
+        <v>28.08863200000001</v>
       </c>
       <c r="E20">
         <v>-0.002376</v>
@@ -7305,7 +7305,7 @@
         <v>-11.883168</v>
       </c>
       <c r="D21">
-        <v>-2.1</v>
+        <v>8.049888000000001</v>
       </c>
       <c r="E21">
         <v>-0.001364</v>
@@ -7322,7 +7322,7 @@
         <v>-23.822524</v>
       </c>
       <c r="D22">
-        <v>-1.3125</v>
+        <v>13.520892</v>
       </c>
       <c r="E22">
         <v>-0.001628</v>
@@ -7339,7 +7339,7 @@
         <v>-12.95866</v>
       </c>
       <c r="D23">
-        <v>-1.5</v>
+        <v>7.775195999999999</v>
       </c>
       <c r="E23">
         <v>-0.00286</v>
@@ -7373,7 +7373,7 @@
         <v>-19.388512</v>
       </c>
       <c r="D25">
-        <v>-0.6774193548387096</v>
+        <v>7.829976</v>
       </c>
       <c r="E25">
         <v>-0.002288</v>
@@ -7390,7 +7390,7 @@
         <v>-41.12768</v>
       </c>
       <c r="D26">
-        <v>-0.1594202898550723</v>
+        <v>5.655055999999995</v>
       </c>
       <c r="E26">
         <v>-0.00352</v>
@@ -7407,7 +7407,7 @@
         <v>-26.540976</v>
       </c>
       <c r="D27">
-        <v>-1.205128205128205</v>
+        <v>14.504952</v>
       </c>
       <c r="E27">
         <v>-0.003784</v>
@@ -7424,7 +7424,7 @@
         <v>-15.907408</v>
       </c>
       <c r="D28">
-        <v>-0.6341463414634148</v>
+        <v>6.173024000000002</v>
       </c>
       <c r="E28">
         <v>-0.002948000000000001</v>
@@ -7441,7 +7441,7 @@
         <v>-852.2064180852415</v>
       </c>
       <c r="D29">
-        <v>-0.03188001380515076</v>
+        <v>26.32898399999999</v>
       </c>
       <c r="E29">
         <v>-0.2577756860511922</v>
@@ -7458,7 +7458,7 @@
         <v>-30.21583495692438</v>
       </c>
       <c r="D30">
-        <v>-0.07105497481489011</v>
+        <v>2.004552</v>
       </c>
       <c r="E30">
         <v>-0.001326477674916562</v>
@@ -7475,7 +7475,7 @@
         <v>-1368.31363488054</v>
       </c>
       <c r="D31">
-        <v>-0.06884390701730597</v>
+        <v>88.13265999999999</v>
       </c>
       <c r="E31">
         <v>-0.2589051343198751</v>
@@ -7492,7 +7492,7 @@
         <v>-58.54216913375787</v>
       </c>
       <c r="D32">
-        <v>-0.4521127007932517</v>
+        <v>18.227</v>
       </c>
       <c r="E32">
         <v>-0.003533021673733124</v>
@@ -7509,7 +7509,7 @@
         <v>-57.2726</v>
       </c>
       <c r="D33">
-        <v>-2.125</v>
+        <v>38.945368</v>
       </c>
       <c r="E33">
         <v>-0.0022</v>
@@ -7526,7 +7526,7 @@
         <v>-1595.705896601005</v>
       </c>
       <c r="D34">
-        <v>-0.0178459339110966</v>
+        <v>27.977576</v>
       </c>
       <c r="E34">
         <v>-0.1455537623461649</v>
@@ -7543,7 +7543,7 @@
         <v>-99.478368</v>
       </c>
       <c r="D35">
-        <v>-0.35</v>
+        <v>25.790688</v>
       </c>
       <c r="E35">
         <v>-0.002376</v>
@@ -7560,7 +7560,7 @@
         <v>-360.8119933800868</v>
       </c>
       <c r="D36">
-        <v>-0.03875806881057077</v>
+        <v>13.46259199999997</v>
       </c>
       <c r="E36">
         <v>-0.061320869031286</v>
@@ -7577,7 +7577,7 @@
         <v>-2593.850363756761</v>
       </c>
       <c r="D37">
-        <v>-0.0007384387428349768</v>
+        <v>1.913986240121631</v>
       </c>
       <c r="E37">
         <v>-2.612135310933294</v>
@@ -7594,7 +7594,7 @@
         <v>-5113.563704557987</v>
       </c>
       <c r="D38">
-        <v>-0.0003423737077776336</v>
+        <v>1.750150559950271</v>
       </c>
       <c r="E38">
         <v>-5.63167808872025</v>
@@ -7611,7 +7611,7 @@
         <v>-4103.376990046077</v>
       </c>
       <c r="D39">
-        <v>-0.0005597613891979092</v>
+        <v>2.295627000991772</v>
       </c>
       <c r="E39">
         <v>-3.445320730517277</v>
@@ -7628,7 +7628,7 @@
         <v>-2120.418752177013</v>
       </c>
       <c r="D40">
-        <v>-0.0003300789881572605</v>
+        <v>0.6996747282619253</v>
       </c>
       <c r="E40">
         <v>-5.841373972939429</v>
@@ -7645,7 +7645,7 @@
         <v>-5844.334366235004</v>
       </c>
       <c r="D41">
-        <v>-1.879912033592946E-05</v>
+        <v>0.109866279644848</v>
       </c>
       <c r="E41">
         <v>-102.532181863772</v>
@@ -7662,7 +7662,7 @@
         <v>-3114.616011846952</v>
       </c>
       <c r="D42">
-        <v>-0.001548279537737837</v>
+        <v>4.814841518452795</v>
       </c>
       <c r="E42">
         <v>-1.246843879842655</v>
@@ -7679,7 +7679,7 @@
         <v>-2588.829444075217</v>
       </c>
       <c r="D43">
-        <v>-0.000546788769125518</v>
+        <v>1.414769285245711</v>
       </c>
       <c r="E43">
         <v>-3.52701559138313</v>
@@ -7696,7 +7696,7 @@
         <v>-317.7178294279209</v>
       </c>
       <c r="D44">
-        <v>-0.08830657028552776</v>
+        <v>25.78002614463782</v>
       </c>
       <c r="E44">
         <v>-0.02375460406937727</v>
@@ -7713,7 +7713,7 @@
         <v>-12.29673788586199</v>
       </c>
       <c r="D45">
-        <v>-0.2248161119518613</v>
+        <v>2.257077429186609</v>
       </c>
       <c r="E45">
         <v>-0.01050105711858411</v>
@@ -7730,7 +7730,7 @@
         <v>-1446.721599305501</v>
       </c>
       <c r="D46">
-        <v>-0.001709604155387335</v>
+        <v>2.469100074114522</v>
       </c>
       <c r="E46">
         <v>-1.129368929980875</v>
@@ -7747,7 +7747,7 @@
         <v>-3665.603804174589</v>
       </c>
       <c r="D47">
-        <v>-0.003587404947212173</v>
+        <v>13.10299945654197</v>
       </c>
       <c r="E47">
         <v>-0.5392179764893481</v>
@@ -7764,7 +7764,7 @@
         <v>-5017.751472717856</v>
       </c>
       <c r="D48">
-        <v>-0.0009985868200385766</v>
+        <v>5.005661898887411</v>
       </c>
       <c r="E48">
         <v>-1.932133797735023</v>
@@ -7781,7 +7781,7 @@
         <v>-3314.323262046861</v>
       </c>
       <c r="D49">
-        <v>-0.001103272499869052</v>
+        <v>3.652571928530051</v>
       </c>
       <c r="E49">
         <v>-1.748983251739768</v>
@@ -7798,7 +7798,7 @@
         <v>-63017.04909083183</v>
       </c>
       <c r="D50">
-        <v>-2.333813639627347E-05</v>
+        <v>1.470666164364957</v>
       </c>
       <c r="E50">
         <v>-82.59115215050043</v>
@@ -7815,7 +7815,7 @@
         <v>-5031.019218466802</v>
       </c>
       <c r="D51">
-        <v>-0.0005704061130938766</v>
+        <v>2.868088142296983</v>
       </c>
       <c r="E51">
         <v>-3.381061302733066</v>
@@ -7832,7 +7832,7 @@
         <v>-196.0776900088526</v>
       </c>
       <c r="D52">
-        <v>-0.05036677608747721</v>
+        <v>9.40224056325556</v>
       </c>
       <c r="E52">
         <v>-0.04019632841509894</v>
@@ -7849,7 +7849,7 @@
         <v>-8352.819267225961</v>
       </c>
       <c r="D53">
-        <v>-0.0003668087181389147</v>
+        <v>3.062763479911155</v>
       </c>
       <c r="E53">
         <v>-5.256651521224645</v>
@@ -7866,7 +7866,7 @@
         <v>-50.12832</v>
       </c>
       <c r="D54">
-        <v>-0.142857142857143</v>
+        <v>6.266040000000004</v>
       </c>
       <c r="E54">
         <v>-0.002112</v>
@@ -7900,7 +7900,7 @@
         <v>-47.6624567106058</v>
       </c>
       <c r="D56">
-        <v>-0.01112270994620533</v>
+        <v>0.5243040000000008</v>
       </c>
       <c r="E56">
         <v>-0.003999870485952148</v>
@@ -7934,7 +7934,7 @@
         <v>-1.39986</v>
       </c>
       <c r="D58">
-        <v>-0.1666666666666667</v>
+        <v>0.19998</v>
       </c>
       <c r="E58">
         <v>-0.000308</v>
@@ -7951,7 +7951,7 @@
         <v>-41.02943975793094</v>
       </c>
       <c r="D59">
-        <v>-0.3434416912526709</v>
+        <v>10.488896</v>
       </c>
       <c r="E59">
         <v>-0.00275383849640452</v>
@@ -7968,7 +7968,7 @@
         <v>-24.7401</v>
       </c>
       <c r="D60">
-        <v>-0.9230769230769231</v>
+        <v>11.875248</v>
       </c>
       <c r="E60">
         <v>-0.0011</v>
@@ -7985,7 +7985,7 @@
         <v>-139.6454081088867</v>
       </c>
       <c r="D61">
-        <v>-0.3020875258272792</v>
+        <v>32.39808000000001</v>
       </c>
       <c r="E61">
         <v>-0.01213780166092019</v>
@@ -8002,7 +8002,7 @@
         <v>-41.43853794396396</v>
       </c>
       <c r="D62">
-        <v>-0.3191596560349527</v>
+        <v>10.025708</v>
       </c>
       <c r="E62">
         <v>-0.007820067549342134</v>
@@ -8019,7 +8019,7 @@
         <v>-2.21144</v>
       </c>
       <c r="D63">
-        <v>-4</v>
+        <v>1.769152</v>
       </c>
       <c r="E63">
         <v>-0.00044</v>
@@ -8036,7 +8036,7 @@
         <v>-4849.881829873122</v>
       </c>
       <c r="D64">
-        <v>-0.01164540405967473</v>
+        <v>55.8286859446016</v>
       </c>
       <c r="E64">
         <v>-0.2797901136421554</v>
@@ -8053,7 +8053,7 @@
         <v>-46.79773753258728</v>
       </c>
       <c r="D65">
-        <v>-0.2090369988294649</v>
+        <v>8.091115999999992</v>
       </c>
       <c r="E65">
         <v>-0.004326313907052536</v>
@@ -8070,7 +8070,7 @@
         <v>-53.53774734297895</v>
       </c>
       <c r="D66">
-        <v>-0.1215930979002412</v>
+        <v>5.804083999999996</v>
       </c>
       <c r="E66">
         <v>-0.005276214382869709</v>
@@ -8104,7 +8104,7 @@
         <v>-35.20149600000001</v>
       </c>
       <c r="D68">
-        <v>-1.186046511627907</v>
+        <v>19.09868400000001</v>
       </c>
       <c r="E68">
         <v>-0.004136000000000001</v>
@@ -8121,7 +8121,7 @@
         <v>-13.66464</v>
       </c>
       <c r="D69">
-        <v>-2.2</v>
+        <v>9.394439999999999</v>
       </c>
       <c r="E69">
         <v>-0.001408</v>
@@ -8138,7 +8138,7 @@
         <v>-58.76847242677465</v>
       </c>
       <c r="D70">
-        <v>-0.06275550464371213</v>
+        <v>3.470266800000005</v>
       </c>
       <c r="E70">
         <v>-0.008718064445449437</v>
@@ -8155,7 +8155,7 @@
         <v>-147.5012698244545</v>
       </c>
       <c r="D71">
-        <v>-0.3085797449108373</v>
+        <v>34.7826751816001</v>
       </c>
       <c r="E71">
         <v>-0.01010282670030511</v>
@@ -8172,7 +8172,7 @@
         <v>-11.6747350696257</v>
       </c>
       <c r="D72">
-        <v>-2.558442790634336</v>
+        <v>8.393879999999999</v>
       </c>
       <c r="E72">
         <v>-0.001835938837808728</v>
@@ -8189,7 +8189,7 @@
         <v>-17.265248</v>
       </c>
       <c r="D73">
-        <v>-0.05925925925925946</v>
+        <v>0.9658880000000032</v>
       </c>
       <c r="E73">
         <v>-0.006292000000000002</v>
@@ -8206,7 +8206,7 @@
         <v>-73.37063053232468</v>
       </c>
       <c r="D74">
-        <v>-0.1843778066882009</v>
+        <v>11.42196000000001</v>
       </c>
       <c r="E74">
         <v>-0.002826404350411213</v>
@@ -8223,7 +8223,7 @@
         <v>-18.02186825928523</v>
       </c>
       <c r="D75">
-        <v>-0.5223265381902549</v>
+        <v>6.183496</v>
       </c>
       <c r="E75">
         <v>-0.003718916273067525</v>
@@ -8240,7 +8240,7 @@
         <v>-75.88922000000001</v>
       </c>
       <c r="D76">
-        <v>-0.6086956521739133</v>
+        <v>28.71484000000001</v>
       </c>
       <c r="E76">
         <v>-0.008140000000000001</v>
@@ -8257,7 +8257,7 @@
         <v>-36.12285600000001</v>
       </c>
       <c r="D77">
-        <v>-0.4807692307692309</v>
+        <v>11.7282</v>
       </c>
       <c r="E77">
         <v>-0.010164</v>
@@ -8274,7 +8274,7 @@
         <v>-18.494784</v>
       </c>
       <c r="D78">
-        <v>-0.5555555555555555</v>
+        <v>6.605279999999999</v>
       </c>
       <c r="E78">
         <v>-0.003696</v>
@@ -8291,7 +8291,7 @@
         <v>-22.4532</v>
       </c>
       <c r="D79">
-        <v>-0.5000000000000002</v>
+        <v>7.484400000000003</v>
       </c>
       <c r="E79">
         <v>-0.0009240000000000001</v>
@@ -8308,7 +8308,7 @@
         <v>-33.204688</v>
       </c>
       <c r="D80">
-        <v>-0.5102040816326526</v>
+        <v>11.21779999999999</v>
       </c>
       <c r="E80">
         <v>-0.003256</v>
@@ -8325,7 +8325,7 @@
         <v>-65.030152</v>
       </c>
       <c r="D81">
-        <v>-2.106382978723405</v>
+        <v>44.095788</v>
       </c>
       <c r="E81">
         <v>-0.006424</v>
@@ -8342,7 +8342,7 @@
         <v>-43.29419600000001</v>
       </c>
       <c r="D82">
-        <v>-0.1318681318681319</v>
+        <v>5.043984000000002</v>
       </c>
       <c r="E82">
         <v>-0.004532</v>
@@ -8359,7 +8359,7 @@
         <v>-29.180448</v>
       </c>
       <c r="D83">
-        <v>-2.978260869565218</v>
+        <v>21.845472</v>
       </c>
       <c r="E83">
         <v>-0.008052</v>
@@ -8376,7 +8376,7 @@
         <v>-17.5032</v>
       </c>
       <c r="D84">
-        <v>-3.193548387096774</v>
+        <v>13.32936</v>
       </c>
       <c r="E84">
         <v>-0.001144</v>
@@ -8393,7 +8393,7 @@
         <v>-35.27519515598377</v>
       </c>
       <c r="D85">
-        <v>-0.6005178514044393</v>
+        <v>13.23533154244761</v>
       </c>
       <c r="E85">
         <v>-0.002092365807935451</v>
@@ -8410,7 +8410,7 @@
         <v>-31.61136</v>
       </c>
       <c r="D86">
-        <v>-4.714285714285714</v>
+        <v>26.079372</v>
       </c>
       <c r="E86">
         <v>-0.00528</v>
@@ -8427,7 +8427,7 @@
         <v>-37.68268829437467</v>
       </c>
       <c r="D87">
-        <v>-1.264758805225826</v>
+        <v>21.043968</v>
       </c>
       <c r="E87">
         <v>-0.003781883610435033</v>
@@ -8444,7 +8444,7 @@
         <v>-382.6199627071207</v>
       </c>
       <c r="D88">
-        <v>-0.6020272147626272</v>
+        <v>143.785092</v>
       </c>
       <c r="E88">
         <v>-0.09987469660848884</v>

</xml_diff>